<commit_message>
Update MAE-Face model weight.
</commit_message>
<xml_diff>
--- a/Record/22AU-3fold-CV-results.xlsx
+++ b/Record/22AU-3fold-CV-results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PHD\论文写作\ASD-AU数据集\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jyf\PycharmProjects\Hugging-Rain-Man\Record\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B563E9-CBB8-48A3-B057-FEE9E2A0BAA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6F9B63-588D-4E3A-B793-BF5F1B3370EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="2100" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="36">
   <si>
     <t>22个AU算法结果</t>
   </si>
@@ -150,6 +150,10 @@
     <t>stage1</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
+  <si>
+    <t>MAE-FACE-NEW</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -230,7 +234,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -257,6 +261,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -533,15 +543,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S139"/>
+  <dimension ref="A1:W144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="L131" sqref="L131"/>
+    <sheetView tabSelected="1" topLeftCell="C114" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L142" sqref="L142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14"/>
   <cols>
     <col min="2" max="9" width="12.453125"/>
+    <col min="11" max="11" width="11.7265625" customWidth="1"/>
     <col min="12" max="19" width="12.453125"/>
   </cols>
   <sheetData>
@@ -5998,7 +6009,12 @@
         <v>52.278030303030299</v>
       </c>
     </row>
-    <row r="115" spans="2:10">
+    <row r="114" spans="2:23">
+      <c r="V114" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="115" spans="2:23">
       <c r="B115" t="s">
         <v>31</v>
       </c>
@@ -6014,8 +6030,14 @@
         <v>16</v>
       </c>
       <c r="H115" s="8"/>
-    </row>
-    <row r="116" spans="2:10">
+      <c r="V115" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="W115" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="116" spans="2:23">
       <c r="B116" t="s">
         <v>18</v>
       </c>
@@ -6043,8 +6065,41 @@
       <c r="J116" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="117" spans="2:10">
+      <c r="L116" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M116" t="s">
+        <v>5</v>
+      </c>
+      <c r="N116" t="s">
+        <v>6</v>
+      </c>
+      <c r="O116" t="s">
+        <v>5</v>
+      </c>
+      <c r="P116" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q116" t="s">
+        <v>5</v>
+      </c>
+      <c r="R116" t="s">
+        <v>6</v>
+      </c>
+      <c r="S116" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="T116" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="V116" s="5">
+        <v>89.323333333333338</v>
+      </c>
+      <c r="W116" s="5">
+        <v>57.273333333333333</v>
+      </c>
+    </row>
+    <row r="117" spans="2:23">
       <c r="B117">
         <v>1</v>
       </c>
@@ -6074,8 +6129,43 @@
         <f t="shared" si="18"/>
         <v>86.303333333333342</v>
       </c>
-    </row>
-    <row r="118" spans="2:10">
+      <c r="L117">
+        <v>1</v>
+      </c>
+      <c r="M117" s="9">
+        <v>0.61519999999999997</v>
+      </c>
+      <c r="N117" s="9">
+        <v>0.87929999999999997</v>
+      </c>
+      <c r="O117" s="10">
+        <v>0.54359999999999997</v>
+      </c>
+      <c r="P117" s="9">
+        <v>0.89749999999999996</v>
+      </c>
+      <c r="Q117" s="9">
+        <v>0.55940000000000001</v>
+      </c>
+      <c r="R117" s="9">
+        <v>0.90290000000000004</v>
+      </c>
+      <c r="S117" s="10">
+        <f>AVERAGE(M117,O117,Q117)</f>
+        <v>0.57273333333333332</v>
+      </c>
+      <c r="T117" s="10">
+        <f>AVERAGE(N117,P117,R117)</f>
+        <v>0.89323333333333332</v>
+      </c>
+      <c r="V117" s="5">
+        <v>91.696666666666673</v>
+      </c>
+      <c r="W117" s="5">
+        <v>57.546666666666667</v>
+      </c>
+    </row>
+    <row r="118" spans="2:23">
       <c r="B118">
         <v>2</v>
       </c>
@@ -6105,8 +6195,43 @@
         <f t="shared" si="18"/>
         <v>88.42</v>
       </c>
-    </row>
-    <row r="119" spans="2:10">
+      <c r="L118">
+        <v>2</v>
+      </c>
+      <c r="M118" s="10">
+        <v>0.62629999999999997</v>
+      </c>
+      <c r="N118" s="10">
+        <v>0.90800000000000003</v>
+      </c>
+      <c r="O118" s="10">
+        <v>0.54779999999999995</v>
+      </c>
+      <c r="P118" s="10">
+        <v>0.91969999999999996</v>
+      </c>
+      <c r="Q118" s="10">
+        <v>0.55230000000000001</v>
+      </c>
+      <c r="R118" s="10">
+        <v>0.92320000000000002</v>
+      </c>
+      <c r="S118" s="10">
+        <f t="shared" ref="S118:S139" si="19">AVERAGE(M118,O118,Q118)</f>
+        <v>0.57546666666666668</v>
+      </c>
+      <c r="T118" s="10">
+        <f t="shared" ref="T118:T139" si="20">AVERAGE(N118,P118,R118)</f>
+        <v>0.91696666666666671</v>
+      </c>
+      <c r="V118" s="5">
+        <v>93.66</v>
+      </c>
+      <c r="W118" s="5">
+        <v>67.373333333333335</v>
+      </c>
+    </row>
+    <row r="119" spans="2:23">
       <c r="B119">
         <v>4</v>
       </c>
@@ -6136,8 +6261,43 @@
         <f t="shared" si="18"/>
         <v>92.086666666666659</v>
       </c>
-    </row>
-    <row r="120" spans="2:10">
+      <c r="L119">
+        <v>4</v>
+      </c>
+      <c r="M119" s="10">
+        <v>0.67659999999999998</v>
+      </c>
+      <c r="N119" s="10">
+        <v>0.93669999999999998</v>
+      </c>
+      <c r="O119" s="10">
+        <v>0.65620000000000001</v>
+      </c>
+      <c r="P119" s="10">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="Q119" s="10">
+        <v>0.68840000000000001</v>
+      </c>
+      <c r="R119" s="10">
+        <v>0.93510000000000004</v>
+      </c>
+      <c r="S119" s="10">
+        <f t="shared" si="19"/>
+        <v>0.6737333333333333</v>
+      </c>
+      <c r="T119" s="10">
+        <f t="shared" si="20"/>
+        <v>0.93659999999999999</v>
+      </c>
+      <c r="V119" s="5">
+        <v>93.596666666666678</v>
+      </c>
+      <c r="W119" s="5">
+        <v>61.720000000000006</v>
+      </c>
+    </row>
+    <row r="120" spans="2:23">
       <c r="B120">
         <v>6</v>
       </c>
@@ -6167,8 +6327,43 @@
         <f t="shared" si="18"/>
         <v>91.75333333333333</v>
       </c>
-    </row>
-    <row r="121" spans="2:10">
+      <c r="L120">
+        <v>6</v>
+      </c>
+      <c r="M120" s="10">
+        <v>0.5726</v>
+      </c>
+      <c r="N120" s="10">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="O120" s="10">
+        <v>0.62990000000000002</v>
+      </c>
+      <c r="P120" s="9">
+        <v>0.93330000000000002</v>
+      </c>
+      <c r="Q120" s="10">
+        <v>0.64910000000000001</v>
+      </c>
+      <c r="R120" s="10">
+        <v>0.9456</v>
+      </c>
+      <c r="S120" s="10">
+        <f t="shared" si="19"/>
+        <v>0.61720000000000008</v>
+      </c>
+      <c r="T120" s="10">
+        <f t="shared" si="20"/>
+        <v>0.93596666666666672</v>
+      </c>
+      <c r="V120" s="5">
+        <v>91.64</v>
+      </c>
+      <c r="W120" s="5">
+        <v>71.709999999999994</v>
+      </c>
+    </row>
+    <row r="121" spans="2:23">
       <c r="B121">
         <v>7</v>
       </c>
@@ -6198,8 +6393,43 @@
         <f t="shared" si="18"/>
         <v>89.286666666666676</v>
       </c>
-    </row>
-    <row r="122" spans="2:10">
+      <c r="L121">
+        <v>7</v>
+      </c>
+      <c r="M121" s="10">
+        <v>0.67120000000000002</v>
+      </c>
+      <c r="N121" s="10">
+        <v>0.90580000000000005</v>
+      </c>
+      <c r="O121" s="10">
+        <v>0.73070000000000002</v>
+      </c>
+      <c r="P121" s="10">
+        <v>0.93259999999999998</v>
+      </c>
+      <c r="Q121" s="10">
+        <v>0.74939999999999996</v>
+      </c>
+      <c r="R121" s="10">
+        <v>0.91080000000000005</v>
+      </c>
+      <c r="S121" s="10">
+        <f t="shared" si="19"/>
+        <v>0.71709999999999996</v>
+      </c>
+      <c r="T121" s="10">
+        <f t="shared" si="20"/>
+        <v>0.91639999999999999</v>
+      </c>
+      <c r="V121" s="5">
+        <v>99.076666666666654</v>
+      </c>
+      <c r="W121" s="5">
+        <v>57.499999999999993</v>
+      </c>
+    </row>
+    <row r="122" spans="2:23">
       <c r="B122">
         <v>9</v>
       </c>
@@ -6229,8 +6459,43 @@
         <f t="shared" si="18"/>
         <v>98.736666666666665</v>
       </c>
-    </row>
-    <row r="123" spans="2:10">
+      <c r="L122">
+        <v>9</v>
+      </c>
+      <c r="M122" s="10">
+        <v>0.61019999999999996</v>
+      </c>
+      <c r="N122" s="10">
+        <v>0.98909999999999998</v>
+      </c>
+      <c r="O122" s="10">
+        <v>0.49559999999999998</v>
+      </c>
+      <c r="P122" s="10">
+        <v>0.98960000000000004</v>
+      </c>
+      <c r="Q122" s="10">
+        <v>0.61919999999999997</v>
+      </c>
+      <c r="R122" s="10">
+        <v>0.99360000000000004</v>
+      </c>
+      <c r="S122" s="10">
+        <f t="shared" si="19"/>
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="T122" s="10">
+        <f t="shared" si="20"/>
+        <v>0.99076666666666657</v>
+      </c>
+      <c r="V122" s="5">
+        <v>93.13</v>
+      </c>
+      <c r="W122" s="5">
+        <v>26.970000000000006</v>
+      </c>
+    </row>
+    <row r="123" spans="2:23">
       <c r="B123">
         <v>10</v>
       </c>
@@ -6260,8 +6525,43 @@
         <f t="shared" si="18"/>
         <v>92.256666666666661</v>
       </c>
-    </row>
-    <row r="124" spans="2:10">
+      <c r="L123">
+        <v>10</v>
+      </c>
+      <c r="M123" s="10">
+        <v>0.29570000000000002</v>
+      </c>
+      <c r="N123" s="10">
+        <v>0.93730000000000002</v>
+      </c>
+      <c r="O123" s="10">
+        <v>0.2177</v>
+      </c>
+      <c r="P123" s="10">
+        <v>0.93769999999999998</v>
+      </c>
+      <c r="Q123" s="10">
+        <v>0.29570000000000002</v>
+      </c>
+      <c r="R123" s="10">
+        <v>0.91890000000000005</v>
+      </c>
+      <c r="S123" s="10">
+        <f t="shared" si="19"/>
+        <v>0.26970000000000005</v>
+      </c>
+      <c r="T123" s="10">
+        <f t="shared" si="20"/>
+        <v>0.93129999999999991</v>
+      </c>
+      <c r="V123" s="5">
+        <v>92.356666666666669</v>
+      </c>
+      <c r="W123" s="5">
+        <v>84.706666666666663</v>
+      </c>
+    </row>
+    <row r="124" spans="2:23">
       <c r="B124">
         <v>12</v>
       </c>
@@ -6291,8 +6591,43 @@
         <f t="shared" si="18"/>
         <v>90.06</v>
       </c>
-    </row>
-    <row r="125" spans="2:10">
+      <c r="L124">
+        <v>12</v>
+      </c>
+      <c r="M124" s="10">
+        <v>0.83979999999999999</v>
+      </c>
+      <c r="N124" s="10">
+        <v>0.91539999999999999</v>
+      </c>
+      <c r="O124" s="10">
+        <v>0.85519999999999996</v>
+      </c>
+      <c r="P124" s="10">
+        <v>0.92520000000000002</v>
+      </c>
+      <c r="Q124" s="10">
+        <v>0.84619999999999995</v>
+      </c>
+      <c r="R124" s="10">
+        <v>0.93010000000000004</v>
+      </c>
+      <c r="S124" s="10">
+        <f t="shared" si="19"/>
+        <v>0.84706666666666663</v>
+      </c>
+      <c r="T124" s="10">
+        <f t="shared" si="20"/>
+        <v>0.92356666666666676</v>
+      </c>
+      <c r="V124" s="5">
+        <v>90.600000000000009</v>
+      </c>
+      <c r="W124" s="5">
+        <v>61.466666666666661</v>
+      </c>
+    </row>
+    <row r="125" spans="2:23">
       <c r="B125">
         <v>14</v>
       </c>
@@ -6322,8 +6657,43 @@
         <f t="shared" si="18"/>
         <v>87.983333333333348</v>
       </c>
-    </row>
-    <row r="126" spans="2:10">
+      <c r="L125">
+        <v>14</v>
+      </c>
+      <c r="M125" s="10">
+        <v>0.71940000000000004</v>
+      </c>
+      <c r="N125" s="10">
+        <v>0.91390000000000005</v>
+      </c>
+      <c r="O125" s="10">
+        <v>0.54930000000000001</v>
+      </c>
+      <c r="P125" s="10">
+        <v>0.91049999999999998</v>
+      </c>
+      <c r="Q125" s="10">
+        <v>0.57530000000000003</v>
+      </c>
+      <c r="R125" s="10">
+        <v>0.89359999999999995</v>
+      </c>
+      <c r="S125" s="10">
+        <f t="shared" si="19"/>
+        <v>0.61466666666666658</v>
+      </c>
+      <c r="T125" s="10">
+        <f t="shared" si="20"/>
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="V125" s="5">
+        <v>99.429999999999993</v>
+      </c>
+      <c r="W125" s="5">
+        <v>5.8633333333333333</v>
+      </c>
+    </row>
+    <row r="126" spans="2:23">
       <c r="B126">
         <v>15</v>
       </c>
@@ -6353,8 +6723,43 @@
         <f t="shared" si="18"/>
         <v>99.453333333333333</v>
       </c>
-    </row>
-    <row r="127" spans="2:10">
+      <c r="L126">
+        <v>15</v>
+      </c>
+      <c r="M126" s="10">
+        <v>0</v>
+      </c>
+      <c r="N126" s="10">
+        <v>0.996</v>
+      </c>
+      <c r="O126" s="10">
+        <v>9.8799999999999999E-2</v>
+      </c>
+      <c r="P126" s="10">
+        <v>0.99260000000000004</v>
+      </c>
+      <c r="Q126" s="10">
+        <v>7.7100000000000002E-2</v>
+      </c>
+      <c r="R126" s="10">
+        <v>0.99429999999999996</v>
+      </c>
+      <c r="S126" s="10">
+        <f t="shared" si="19"/>
+        <v>5.8633333333333336E-2</v>
+      </c>
+      <c r="T126" s="10">
+        <f t="shared" si="20"/>
+        <v>0.99429999999999996</v>
+      </c>
+      <c r="V126" s="5">
+        <v>93.483333333333334</v>
+      </c>
+      <c r="W126" s="5">
+        <v>27.513333333333335</v>
+      </c>
+    </row>
+    <row r="127" spans="2:23">
       <c r="B127">
         <v>16</v>
       </c>
@@ -6384,8 +6789,43 @@
         <f t="shared" si="18"/>
         <v>93.04</v>
       </c>
-    </row>
-    <row r="128" spans="2:10">
+      <c r="L127">
+        <v>16</v>
+      </c>
+      <c r="M127" s="10">
+        <v>0.3276</v>
+      </c>
+      <c r="N127" s="10">
+        <v>0.90759999999999996</v>
+      </c>
+      <c r="O127" s="10">
+        <v>0.157</v>
+      </c>
+      <c r="P127" s="10">
+        <v>0.93830000000000002</v>
+      </c>
+      <c r="Q127" s="10">
+        <v>0.34079999999999999</v>
+      </c>
+      <c r="R127" s="10">
+        <v>0.95860000000000001</v>
+      </c>
+      <c r="S127" s="10">
+        <f t="shared" si="19"/>
+        <v>0.27513333333333334</v>
+      </c>
+      <c r="T127" s="10">
+        <f t="shared" si="20"/>
+        <v>0.93483333333333329</v>
+      </c>
+      <c r="V127" s="5">
+        <v>96.023333333333341</v>
+      </c>
+      <c r="W127" s="5">
+        <v>47.923333333333332</v>
+      </c>
+    </row>
+    <row r="128" spans="2:23">
       <c r="B128">
         <v>17</v>
       </c>
@@ -6415,8 +6855,43 @@
         <f t="shared" si="18"/>
         <v>95.043333333333337</v>
       </c>
-    </row>
-    <row r="129" spans="2:10">
+      <c r="L128">
+        <v>17</v>
+      </c>
+      <c r="M128" s="10">
+        <v>0.49740000000000001</v>
+      </c>
+      <c r="N128" s="10">
+        <v>0.96950000000000003</v>
+      </c>
+      <c r="O128" s="10">
+        <v>0.50639999999999996</v>
+      </c>
+      <c r="P128" s="10">
+        <v>0.95660000000000001</v>
+      </c>
+      <c r="Q128" s="10">
+        <v>0.43390000000000001</v>
+      </c>
+      <c r="R128" s="10">
+        <v>0.9546</v>
+      </c>
+      <c r="S128" s="10">
+        <f t="shared" si="19"/>
+        <v>0.47923333333333334</v>
+      </c>
+      <c r="T128" s="10">
+        <f t="shared" si="20"/>
+        <v>0.96023333333333338</v>
+      </c>
+      <c r="V128" s="5">
+        <v>97.803333333333327</v>
+      </c>
+      <c r="W128" s="5">
+        <v>52.293333333333337</v>
+      </c>
+    </row>
+    <row r="129" spans="2:23">
       <c r="B129">
         <v>18</v>
       </c>
@@ -6446,8 +6921,43 @@
         <f t="shared" si="18"/>
         <v>97.38666666666667</v>
       </c>
-    </row>
-    <row r="130" spans="2:10">
+      <c r="L129">
+        <v>18</v>
+      </c>
+      <c r="M129" s="10">
+        <v>0.42170000000000002</v>
+      </c>
+      <c r="N129" s="10">
+        <v>0.98040000000000005</v>
+      </c>
+      <c r="O129" s="10">
+        <v>0.59740000000000004</v>
+      </c>
+      <c r="P129" s="10">
+        <v>0.97009999999999996</v>
+      </c>
+      <c r="Q129" s="10">
+        <v>0.54969999999999997</v>
+      </c>
+      <c r="R129" s="10">
+        <v>0.98360000000000003</v>
+      </c>
+      <c r="S129" s="10">
+        <f t="shared" si="19"/>
+        <v>0.52293333333333336</v>
+      </c>
+      <c r="T129" s="10">
+        <f t="shared" si="20"/>
+        <v>0.97803333333333331</v>
+      </c>
+      <c r="V129" s="5">
+        <v>98.993333333333325</v>
+      </c>
+      <c r="W129" s="5">
+        <v>70.793333333333337</v>
+      </c>
+    </row>
+    <row r="130" spans="2:23">
       <c r="B130">
         <v>19</v>
       </c>
@@ -6477,8 +6987,43 @@
         <f t="shared" si="18"/>
         <v>98.46</v>
       </c>
-    </row>
-    <row r="131" spans="2:10">
+      <c r="L130">
+        <v>19</v>
+      </c>
+      <c r="M130" s="10">
+        <v>0.6089</v>
+      </c>
+      <c r="N130" s="10">
+        <v>0.99219999999999997</v>
+      </c>
+      <c r="O130" s="10">
+        <v>0.77170000000000005</v>
+      </c>
+      <c r="P130" s="10">
+        <v>0.98229999999999995</v>
+      </c>
+      <c r="Q130" s="10">
+        <v>0.74319999999999997</v>
+      </c>
+      <c r="R130" s="10">
+        <v>0.99529999999999996</v>
+      </c>
+      <c r="S130" s="10">
+        <f t="shared" si="19"/>
+        <v>0.70793333333333341</v>
+      </c>
+      <c r="T130" s="10">
+        <f t="shared" si="20"/>
+        <v>0.98993333333333322</v>
+      </c>
+      <c r="V130" s="5">
+        <v>97.626666666666665</v>
+      </c>
+      <c r="W130" s="5">
+        <v>41.053333333333335</v>
+      </c>
+    </row>
+    <row r="131" spans="2:23">
       <c r="B131">
         <v>20</v>
       </c>
@@ -6508,8 +7053,43 @@
         <f t="shared" si="18"/>
         <v>97.21</v>
       </c>
-    </row>
-    <row r="132" spans="2:10">
+      <c r="L131">
+        <v>20</v>
+      </c>
+      <c r="M131" s="10">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="N131" s="10">
+        <v>0.96640000000000004</v>
+      </c>
+      <c r="O131" s="10">
+        <v>0.40279999999999999</v>
+      </c>
+      <c r="P131" s="10">
+        <v>0.97529999999999994</v>
+      </c>
+      <c r="Q131" s="10">
+        <v>0.4178</v>
+      </c>
+      <c r="R131" s="10">
+        <v>0.98709999999999998</v>
+      </c>
+      <c r="S131" s="10">
+        <f t="shared" si="19"/>
+        <v>0.41053333333333336</v>
+      </c>
+      <c r="T131" s="10">
+        <f t="shared" si="20"/>
+        <v>0.97626666666666662</v>
+      </c>
+      <c r="V131" s="5">
+        <v>95.223333333333343</v>
+      </c>
+      <c r="W131" s="5">
+        <v>26.153333333333332</v>
+      </c>
+    </row>
+    <row r="132" spans="2:23">
       <c r="B132">
         <v>23</v>
       </c>
@@ -6539,8 +7119,43 @@
         <f t="shared" si="18"/>
         <v>94.240000000000009</v>
       </c>
-    </row>
-    <row r="133" spans="2:10">
+      <c r="L132">
+        <v>23</v>
+      </c>
+      <c r="M132" s="10">
+        <v>0.29980000000000001</v>
+      </c>
+      <c r="N132" s="10">
+        <v>0.9536</v>
+      </c>
+      <c r="O132" s="10">
+        <v>0.21859999999999999</v>
+      </c>
+      <c r="P132" s="10">
+        <v>0.95379999999999998</v>
+      </c>
+      <c r="Q132" s="10">
+        <v>0.26619999999999999</v>
+      </c>
+      <c r="R132" s="10">
+        <v>0.94930000000000003</v>
+      </c>
+      <c r="S132" s="10">
+        <f t="shared" si="19"/>
+        <v>0.26153333333333334</v>
+      </c>
+      <c r="T132" s="10">
+        <f t="shared" si="20"/>
+        <v>0.95223333333333338</v>
+      </c>
+      <c r="V132" s="5">
+        <v>95.936666666666653</v>
+      </c>
+      <c r="W132" s="5">
+        <v>36.136666666666663</v>
+      </c>
+    </row>
+    <row r="133" spans="2:23">
       <c r="B133">
         <v>24</v>
       </c>
@@ -6570,8 +7185,43 @@
         <f t="shared" si="18"/>
         <v>94.893333333333331</v>
       </c>
-    </row>
-    <row r="134" spans="2:10">
+      <c r="L133">
+        <v>24</v>
+      </c>
+      <c r="M133" s="10">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="N133" s="10">
+        <v>0.96460000000000001</v>
+      </c>
+      <c r="O133" s="10">
+        <v>0.2974</v>
+      </c>
+      <c r="P133" s="10">
+        <v>0.95879999999999999</v>
+      </c>
+      <c r="Q133" s="10">
+        <v>0.32369999999999999</v>
+      </c>
+      <c r="R133" s="10">
+        <v>0.95469999999999999</v>
+      </c>
+      <c r="S133" s="10">
+        <f t="shared" si="19"/>
+        <v>0.36136666666666661</v>
+      </c>
+      <c r="T133" s="10">
+        <f t="shared" si="20"/>
+        <v>0.95936666666666659</v>
+      </c>
+      <c r="V133" s="5">
+        <v>93.043333333333322</v>
+      </c>
+      <c r="W133" s="5">
+        <v>94.749999999999986</v>
+      </c>
+    </row>
+    <row r="134" spans="2:23">
       <c r="B134">
         <v>25</v>
       </c>
@@ -6601,8 +7251,43 @@
         <f t="shared" si="18"/>
         <v>89.576666666666668</v>
       </c>
-    </row>
-    <row r="135" spans="2:10">
+      <c r="L134">
+        <v>25</v>
+      </c>
+      <c r="M134" s="10">
+        <v>0.93340000000000001</v>
+      </c>
+      <c r="N134" s="10">
+        <v>0.91879999999999995</v>
+      </c>
+      <c r="O134" s="10">
+        <v>0.95609999999999995</v>
+      </c>
+      <c r="P134" s="10">
+        <v>0.93469999999999998</v>
+      </c>
+      <c r="Q134" s="10">
+        <v>0.95299999999999996</v>
+      </c>
+      <c r="R134" s="10">
+        <v>0.93779999999999997</v>
+      </c>
+      <c r="S134" s="10">
+        <f t="shared" si="19"/>
+        <v>0.9474999999999999</v>
+      </c>
+      <c r="T134" s="10">
+        <f t="shared" si="20"/>
+        <v>0.93043333333333322</v>
+      </c>
+      <c r="V134" s="5">
+        <v>81.16</v>
+      </c>
+      <c r="W134" s="5">
+        <v>76.516666666666666</v>
+      </c>
+    </row>
+    <row r="135" spans="2:23">
       <c r="B135">
         <v>27</v>
       </c>
@@ -6632,8 +7317,43 @@
         <f t="shared" si="18"/>
         <v>75.570000000000007</v>
       </c>
-    </row>
-    <row r="136" spans="2:10">
+      <c r="L135">
+        <v>27</v>
+      </c>
+      <c r="M135" s="10">
+        <v>0.73070000000000002</v>
+      </c>
+      <c r="N135" s="10">
+        <v>0.80979999999999996</v>
+      </c>
+      <c r="O135" s="10">
+        <v>0.77329999999999999</v>
+      </c>
+      <c r="P135" s="10">
+        <v>0.81589999999999996</v>
+      </c>
+      <c r="Q135" s="10">
+        <v>0.79149999999999998</v>
+      </c>
+      <c r="R135" s="10">
+        <v>0.80910000000000004</v>
+      </c>
+      <c r="S135" s="10">
+        <f t="shared" si="19"/>
+        <v>0.76516666666666666</v>
+      </c>
+      <c r="T135" s="10">
+        <f t="shared" si="20"/>
+        <v>0.81159999999999999</v>
+      </c>
+      <c r="V135" s="5">
+        <v>97.63666666666667</v>
+      </c>
+      <c r="W135" s="5">
+        <v>52.030000000000008</v>
+      </c>
+    </row>
+    <row r="136" spans="2:23">
       <c r="B136">
         <v>28</v>
       </c>
@@ -6663,8 +7383,43 @@
         <f t="shared" si="18"/>
         <v>97.516666666666666</v>
       </c>
-    </row>
-    <row r="137" spans="2:10">
+      <c r="L136">
+        <v>28</v>
+      </c>
+      <c r="M136" s="10">
+        <v>0.48420000000000002</v>
+      </c>
+      <c r="N136" s="10">
+        <v>0.97119999999999995</v>
+      </c>
+      <c r="O136" s="10">
+        <v>0.4904</v>
+      </c>
+      <c r="P136" s="10">
+        <v>0.9728</v>
+      </c>
+      <c r="Q136" s="10">
+        <v>0.58630000000000004</v>
+      </c>
+      <c r="R136" s="10">
+        <v>0.98509999999999998</v>
+      </c>
+      <c r="S136" s="10">
+        <f t="shared" si="19"/>
+        <v>0.5203000000000001</v>
+      </c>
+      <c r="T136" s="10">
+        <f t="shared" si="20"/>
+        <v>0.97636666666666672</v>
+      </c>
+      <c r="V136" s="5">
+        <v>98.906666666666666</v>
+      </c>
+      <c r="W136" s="5">
+        <v>50.593333333333327</v>
+      </c>
+    </row>
+    <row r="137" spans="2:23">
       <c r="B137">
         <v>32</v>
       </c>
@@ -6694,8 +7449,43 @@
         <f t="shared" si="18"/>
         <v>98.823333333333338</v>
       </c>
-    </row>
-    <row r="138" spans="2:10">
+      <c r="L137">
+        <v>32</v>
+      </c>
+      <c r="M137" s="10">
+        <v>0.65159999999999996</v>
+      </c>
+      <c r="N137" s="10">
+        <v>0.99250000000000005</v>
+      </c>
+      <c r="O137" s="10">
+        <v>0.37780000000000002</v>
+      </c>
+      <c r="P137" s="10">
+        <v>0.98109999999999997</v>
+      </c>
+      <c r="Q137" s="10">
+        <v>0.4884</v>
+      </c>
+      <c r="R137" s="10">
+        <v>0.99360000000000004</v>
+      </c>
+      <c r="S137" s="10">
+        <f t="shared" si="19"/>
+        <v>0.50593333333333323</v>
+      </c>
+      <c r="T137" s="10">
+        <f t="shared" si="20"/>
+        <v>0.98906666666666665</v>
+      </c>
+      <c r="V137" s="5">
+        <v>98.746666666666655</v>
+      </c>
+      <c r="W137" s="5">
+        <v>70.573333333333338</v>
+      </c>
+    </row>
+    <row r="138" spans="2:23">
       <c r="B138">
         <v>43</v>
       </c>
@@ -6725,33 +7515,68 @@
         <f t="shared" si="18"/>
         <v>97.84333333333332</v>
       </c>
-    </row>
-    <row r="139" spans="2:10">
+      <c r="L138">
+        <v>43</v>
+      </c>
+      <c r="M138" s="10">
+        <v>0.57909999999999995</v>
+      </c>
+      <c r="N138" s="10">
+        <v>0.98719999999999997</v>
+      </c>
+      <c r="O138" s="10">
+        <v>0.75919999999999999</v>
+      </c>
+      <c r="P138" s="10">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="Q138" s="10">
+        <v>0.77890000000000004</v>
+      </c>
+      <c r="R138" s="10">
+        <v>0.98419999999999996</v>
+      </c>
+      <c r="S138" s="10">
+        <f t="shared" si="19"/>
+        <v>0.70573333333333332</v>
+      </c>
+      <c r="T138" s="10">
+        <f t="shared" si="20"/>
+        <v>0.9874666666666666</v>
+      </c>
+      <c r="V138" s="5">
+        <v>94.50424242424242</v>
+      </c>
+      <c r="W138" s="5">
+        <v>54.475454545454539</v>
+      </c>
+    </row>
+    <row r="139" spans="2:23">
       <c r="B139" t="s">
         <v>10</v>
       </c>
       <c r="C139">
-        <f t="shared" ref="C139:H139" si="19">AVERAGE(C117:C138)</f>
+        <f t="shared" ref="C139:H139" si="21">AVERAGE(C117:C138)</f>
         <v>50.379545454545458</v>
       </c>
       <c r="D139">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>92.778181818181793</v>
       </c>
       <c r="E139">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>52.732727272727267</v>
       </c>
       <c r="F139">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>93.158636363636347</v>
       </c>
       <c r="G139">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>49.839090909090913</v>
       </c>
       <c r="H139">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>93.055454545454538</v>
       </c>
       <c r="I139">
@@ -6762,14 +7587,54 @@
         <f t="shared" si="18"/>
         <v>92.997424242424231</v>
       </c>
+      <c r="L139" t="s">
+        <v>11</v>
+      </c>
+      <c r="M139" s="10">
+        <f>AVERAGE(M117:M138)</f>
+        <v>0.54706363636363642</v>
+      </c>
+      <c r="N139" s="10">
+        <f t="shared" ref="M139:R139" si="22">AVERAGE(N117:N138)</f>
+        <v>0.94201363636363655</v>
+      </c>
+      <c r="O139" s="10">
+        <f t="shared" si="22"/>
+        <v>0.52876818181818186</v>
+      </c>
+      <c r="P139" s="10">
+        <f t="shared" si="22"/>
+        <v>0.94579090909090913</v>
+      </c>
+      <c r="Q139" s="10">
+        <f>AVERAGE(Q117:Q138)</f>
+        <v>0.55843181818181808</v>
+      </c>
+      <c r="R139" s="10">
+        <f t="shared" si="22"/>
+        <v>0.94732272727272715</v>
+      </c>
+      <c r="S139" s="10">
+        <f t="shared" si="19"/>
+        <v>0.54475454545454538</v>
+      </c>
+      <c r="T139" s="10">
+        <f t="shared" si="20"/>
+        <v>0.94504242424242424</v>
+      </c>
+    </row>
+    <row r="142" spans="2:23">
+      <c r="L142" s="4"/>
+    </row>
+    <row r="143" spans="2:23">
+      <c r="K143" s="4"/>
+      <c r="L143" s="4"/>
+    </row>
+    <row r="144" spans="2:23">
+      <c r="L144" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="L59:M59"/>
-    <mergeCell ref="N59:O59"/>
     <mergeCell ref="C115:D115"/>
     <mergeCell ref="E115:F115"/>
     <mergeCell ref="G115:H115"/>
@@ -6786,6 +7651,11 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="P59:Q59"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="L59:M59"/>
+    <mergeCell ref="N59:O59"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>